<commit_message>
Small adjustments to a line of code
</commit_message>
<xml_diff>
--- a/Outputs/Tables/Stats_Grouped.xlsx
+++ b/Outputs/Tables/Stats_Grouped.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t xml:space="preserve">2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Untreated</t>
   </si>
   <si>
     <t xml:space="preserve">Control, leisure and parallel</t>
@@ -395,16 +392,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>8.2</v>
+        <v>-26.4</v>
       </c>
       <c r="C2" t="n">
-        <v>28.85</v>
+        <v>-17.5</v>
       </c>
       <c r="D2" t="n">
-        <v>31.3</v>
+        <v>-13.45</v>
       </c>
       <c r="E2" t="n">
-        <v>32.29</v>
+        <v>-13.42</v>
       </c>
     </row>
     <row r="3">
@@ -412,16 +409,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>-26.23</v>
+        <v>-25.16</v>
       </c>
       <c r="C3" t="n">
-        <v>-17.39</v>
+        <v>-10.26</v>
       </c>
       <c r="D3" t="n">
-        <v>-13.34</v>
+        <v>-1.39</v>
       </c>
       <c r="E3" t="n">
-        <v>-13.29</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="4">
@@ -429,16 +426,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>-24.9</v>
+        <v>-29.03</v>
       </c>
       <c r="C4" t="n">
-        <v>-10.08</v>
+        <v>-13.59</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.18</v>
+        <v>-2.67</v>
       </c>
       <c r="E4" t="n">
-        <v>2.01</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="5">
@@ -446,32 +443,15 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>-28.75</v>
+        <v>-28.69</v>
       </c>
       <c r="C5" t="n">
-        <v>-13.39</v>
+        <v>-30.92</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.45</v>
+        <v>-35.81</v>
       </c>
       <c r="E5" t="n">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-28.69</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-30.92</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-35.81</v>
-      </c>
-      <c r="E6" t="n">
         <v>-35.77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected spelling mistake to a string in Untreated group name
</commit_message>
<xml_diff>
--- a/Outputs/Tables/Stats_Grouped.xlsx
+++ b/Outputs/Tables/Stats_Grouped.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t xml:space="preserve">2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Untreated</t>
   </si>
   <si>
     <t xml:space="preserve">Control, leisure and parallel</t>
@@ -392,16 +395,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>-26.4</v>
+        <v>8.2</v>
       </c>
       <c r="C2" t="n">
-        <v>-17.5</v>
+        <v>28.85</v>
       </c>
       <c r="D2" t="n">
-        <v>-13.45</v>
+        <v>31.3</v>
       </c>
       <c r="E2" t="n">
-        <v>-13.42</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="3">
@@ -409,16 +412,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>-25.16</v>
+        <v>-26.4</v>
       </c>
       <c r="C3" t="n">
-        <v>-10.26</v>
+        <v>-17.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.39</v>
+        <v>-13.45</v>
       </c>
       <c r="E3" t="n">
-        <v>1.75</v>
+        <v>-13.42</v>
       </c>
     </row>
     <row r="4">
@@ -426,16 +429,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>-29.03</v>
+        <v>-25.16</v>
       </c>
       <c r="C4" t="n">
-        <v>-13.59</v>
+        <v>-10.26</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.67</v>
+        <v>-1.39</v>
       </c>
       <c r="E4" t="n">
-        <v>2.61</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="5">
@@ -443,15 +446,32 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
+        <v>-29.03</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-13.59</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2.67</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
         <v>-28.69</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>-30.92</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>-35.81</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>-35.77</v>
       </c>
     </row>

</xml_diff>